<commit_message>
08.01.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2019/Others/IMEI.xlsx
+++ b/2019/Others/IMEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2019\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93815584-5634-4CF0-9D4E-17EE5496FC92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F530A-B40F-404B-B576-6866A2826CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="1080" windowWidth="11205" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>